<commit_message>
Updated category select xpath
</commit_message>
<xml_diff>
--- a/items_to_sell.xlsx
+++ b/items_to_sell.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Listing Title</t>
   </si>
@@ -28,22 +28,16 @@
     <t>Description</t>
   </si>
   <si>
-    <t>【啟思】啟思新高中中國語文(第三冊) (2022 第三版)</t>
-  </si>
-  <si>
-    <t>Like new</t>
-  </si>
-  <si>
-    <t>有寫過</t>
-  </si>
-  <si>
-    <t>【啟思】啟思新高中中國語文(第四冊) (2022 第四版)</t>
-  </si>
-  <si>
-    <t>沒有任何筆記highlight</t>
-  </si>
-  <si>
-    <t/>
+    <t>DSE 校園經濟 5蚊一本 有5本</t>
+  </si>
+  <si>
+    <t>Brand new</t>
+  </si>
+  <si>
+    <t>新淨</t>
+  </si>
+  <si>
+    <t>DSE 公社刊物 5 蚊一本 有3本</t>
   </si>
 </sst>
 </file>
@@ -106,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -121,12 +115,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -443,10 +431,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="77.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="42.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="77.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="42.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -471,13 +459,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="4">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -485,95 +473,53 @@
         <v>5</v>
       </c>
       <c r="C3" s="4">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="D4" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="D5" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="D6" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="D7" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="D8" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="D9" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="D10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>